<commit_message>
12 update config, 13 first part
</commit_message>
<xml_diff>
--- a/feste-script/wip_checkliste_gesamt.xlsx
+++ b/feste-script/wip_checkliste_gesamt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://concat-my.sharepoint.com/personal/oliver_antwerpen_concat_de/Documents/Kunden/ITSG/DiGeN/posh/xls-wip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="13_ncr:1_{C0C70AED-9EB6-4CE2-A002-75091045E0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{63ED40BD-D64C-4CF4-B67E-1649A89617F5}"/>
+  <xr:revisionPtr revIDLastSave="190" documentId="13_ncr:1_{C0C70AED-9EB6-4CE2-A002-75091045E0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EFA4D0D9-77CC-4C02-843A-273AA8C315DF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="870" firstSheet="11" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="870" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="26" r:id="rId1"/>
@@ -212,7 +212,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4251" uniqueCount="1767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4259" uniqueCount="1773">
   <si>
     <t>Bitte über "Zellen einfügen" immer eine neue Zeile "5" erstellen! Danke :-)</t>
   </si>
@@ -5704,6 +5704,24 @@
   </si>
   <si>
     <t>disabled</t>
+  </si>
+  <si>
+    <t>Synergy SPP</t>
+  </si>
+  <si>
+    <t>HPE_Synergy_Custom_SPP_2019.03.20190825_Z7550-96751.iso</t>
+  </si>
+  <si>
+    <t>Artifact Bundle</t>
+  </si>
+  <si>
+    <t>HPE-ESXi-6.7-2019-07-24-v4.2.zip</t>
+  </si>
+  <si>
+    <t>Golden Image</t>
+  </si>
+  <si>
+    <t>bla.zip</t>
   </si>
 </sst>
 </file>
@@ -6904,25 +6922,16 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6932,6 +6941,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6944,6 +6956,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -22162,8 +22180,8 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -22580,26 +22598,42 @@
       <c r="G30" s="189"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="6"/>
-      <c r="B31" s="189"/>
+      <c r="A31" s="6" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B31" s="189" t="s">
+        <v>1768</v>
+      </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="189"/>
+      <c r="E31" s="189" t="s">
+        <v>1768</v>
+      </c>
       <c r="F31" s="189"/>
       <c r="G31" s="189"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="6"/>
-      <c r="B32" s="189"/>
+      <c r="A32" s="6" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B32" s="189" t="s">
+        <v>1770</v>
+      </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="189"/>
+      <c r="E32" s="189" t="s">
+        <v>1770</v>
+      </c>
       <c r="F32" s="189"/>
       <c r="G32" s="189"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="6"/>
-      <c r="B33" s="189"/>
+      <c r="A33" s="6" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B33" s="189" t="s">
+        <v>1772</v>
+      </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="189"/>
@@ -23108,7 +23142,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C123FC9F-23EA-4F5F-A4E7-231974F9FE8E}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -24889,16 +24923,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18">
-      <c r="A1" s="199" t="s">
+      <c r="A1" s="201" t="s">
         <v>1280</v>
       </c>
-      <c r="B1" s="200"/>
+      <c r="B1" s="202"/>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="201" t="s">
+      <c r="A2" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="B2" s="202"/>
+      <c r="B2" s="200"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="161" t="s">
@@ -24925,10 +24959,10 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="201" t="s">
+      <c r="A6" s="199" t="s">
         <v>1287</v>
       </c>
-      <c r="B6" s="202"/>
+      <c r="B6" s="200"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="161" t="s">
@@ -24947,10 +24981,10 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="201" t="s">
+      <c r="A9" s="199" t="s">
         <v>1291</v>
       </c>
-      <c r="B9" s="202"/>
+      <c r="B9" s="200"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="161" t="s">
@@ -25002,32 +25036,32 @@
     </row>
     <row r="17" spans="1:9" ht="15" thickBot="1"/>
     <row r="18" spans="1:9" ht="18">
-      <c r="A18" s="199" t="s">
+      <c r="A18" s="201" t="s">
         <v>1302</v>
       </c>
-      <c r="B18" s="205"/>
-      <c r="C18" s="205"/>
-      <c r="D18" s="200"/>
-      <c r="F18" s="199" t="s">
+      <c r="B18" s="206"/>
+      <c r="C18" s="206"/>
+      <c r="D18" s="202"/>
+      <c r="F18" s="201" t="s">
         <v>1302</v>
       </c>
-      <c r="G18" s="205"/>
-      <c r="H18" s="205"/>
-      <c r="I18" s="200"/>
+      <c r="G18" s="206"/>
+      <c r="H18" s="206"/>
+      <c r="I18" s="202"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="201" t="s">
+      <c r="A19" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="B19" s="209"/>
-      <c r="C19" s="209"/>
-      <c r="D19" s="202"/>
-      <c r="F19" s="201" t="s">
+      <c r="B19" s="207"/>
+      <c r="C19" s="207"/>
+      <c r="D19" s="200"/>
+      <c r="F19" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="G19" s="209"/>
-      <c r="H19" s="209"/>
-      <c r="I19" s="202"/>
+      <c r="G19" s="207"/>
+      <c r="H19" s="207"/>
+      <c r="I19" s="200"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="161" t="s">
@@ -25102,88 +25136,88 @@
       <c r="I23" s="162"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="201" t="s">
+      <c r="A24" s="199" t="s">
         <v>1310</v>
       </c>
-      <c r="B24" s="209"/>
-      <c r="C24" s="209"/>
-      <c r="D24" s="202"/>
-      <c r="F24" s="201" t="s">
+      <c r="B24" s="207"/>
+      <c r="C24" s="207"/>
+      <c r="D24" s="200"/>
+      <c r="F24" s="199" t="s">
         <v>1310</v>
       </c>
-      <c r="G24" s="209"/>
-      <c r="H24" s="209"/>
-      <c r="I24" s="202"/>
+      <c r="G24" s="207"/>
+      <c r="H24" s="207"/>
+      <c r="I24" s="200"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="210" t="s">
+      <c r="A25" s="208" t="s">
         <v>1311</v>
       </c>
-      <c r="B25" s="211"/>
-      <c r="C25" s="211"/>
-      <c r="D25" s="212"/>
-      <c r="F25" s="210" t="s">
+      <c r="B25" s="209"/>
+      <c r="C25" s="209"/>
+      <c r="D25" s="210"/>
+      <c r="F25" s="208" t="s">
         <v>1311</v>
       </c>
-      <c r="G25" s="211"/>
-      <c r="H25" s="211"/>
-      <c r="I25" s="212"/>
+      <c r="G25" s="209"/>
+      <c r="H25" s="209"/>
+      <c r="I25" s="210"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="201" t="s">
+      <c r="A26" s="199" t="s">
         <v>1312</v>
       </c>
-      <c r="B26" s="209"/>
-      <c r="C26" s="209"/>
-      <c r="D26" s="202"/>
-      <c r="F26" s="201" t="s">
+      <c r="B26" s="207"/>
+      <c r="C26" s="207"/>
+      <c r="D26" s="200"/>
+      <c r="F26" s="199" t="s">
         <v>1312</v>
       </c>
-      <c r="G26" s="209"/>
-      <c r="H26" s="209"/>
-      <c r="I26" s="202"/>
+      <c r="G26" s="207"/>
+      <c r="H26" s="207"/>
+      <c r="I26" s="200"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="210" t="s">
+      <c r="A27" s="208" t="s">
         <v>1313</v>
       </c>
-      <c r="B27" s="211"/>
-      <c r="C27" s="211"/>
-      <c r="D27" s="212"/>
-      <c r="F27" s="210" t="s">
+      <c r="B27" s="209"/>
+      <c r="C27" s="209"/>
+      <c r="D27" s="210"/>
+      <c r="F27" s="208" t="s">
         <v>1313</v>
       </c>
-      <c r="G27" s="211"/>
-      <c r="H27" s="211"/>
-      <c r="I27" s="212"/>
+      <c r="G27" s="209"/>
+      <c r="H27" s="209"/>
+      <c r="I27" s="210"/>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="201" t="s">
+      <c r="A28" s="199" t="s">
         <v>1314</v>
       </c>
-      <c r="B28" s="209"/>
-      <c r="C28" s="209"/>
-      <c r="D28" s="202"/>
-      <c r="F28" s="201" t="s">
+      <c r="B28" s="207"/>
+      <c r="C28" s="207"/>
+      <c r="D28" s="200"/>
+      <c r="F28" s="199" t="s">
         <v>1314</v>
       </c>
-      <c r="G28" s="209"/>
-      <c r="H28" s="209"/>
-      <c r="I28" s="202"/>
+      <c r="G28" s="207"/>
+      <c r="H28" s="207"/>
+      <c r="I28" s="200"/>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="206" t="s">
+      <c r="A29" s="203" t="s">
         <v>1315</v>
       </c>
-      <c r="B29" s="207"/>
-      <c r="C29" s="207"/>
-      <c r="D29" s="208"/>
-      <c r="F29" s="206" t="s">
+      <c r="B29" s="204"/>
+      <c r="C29" s="204"/>
+      <c r="D29" s="205"/>
+      <c r="F29" s="203" t="s">
         <v>1315</v>
       </c>
-      <c r="G29" s="207"/>
-      <c r="H29" s="207"/>
-      <c r="I29" s="208"/>
+      <c r="G29" s="204"/>
+      <c r="H29" s="204"/>
+      <c r="I29" s="205"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="167" t="s">
@@ -25318,18 +25352,18 @@
       <c r="I35" s="162"/>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="206" t="s">
+      <c r="A36" s="203" t="s">
         <v>1323</v>
       </c>
-      <c r="B36" s="207"/>
-      <c r="C36" s="207"/>
-      <c r="D36" s="208"/>
-      <c r="F36" s="206" t="s">
+      <c r="B36" s="204"/>
+      <c r="C36" s="204"/>
+      <c r="D36" s="205"/>
+      <c r="F36" s="203" t="s">
         <v>1323</v>
       </c>
-      <c r="G36" s="207"/>
-      <c r="H36" s="207"/>
-      <c r="I36" s="208"/>
+      <c r="G36" s="204"/>
+      <c r="H36" s="204"/>
+      <c r="I36" s="205"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="167" t="s">
@@ -25458,18 +25492,18 @@
       <c r="I43" s="162"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="206" t="s">
+      <c r="A44" s="203" t="s">
         <v>1329</v>
       </c>
-      <c r="B44" s="207"/>
-      <c r="C44" s="207"/>
-      <c r="D44" s="208"/>
-      <c r="F44" s="206" t="s">
+      <c r="B44" s="204"/>
+      <c r="C44" s="204"/>
+      <c r="D44" s="205"/>
+      <c r="F44" s="203" t="s">
         <v>1329</v>
       </c>
-      <c r="G44" s="207"/>
-      <c r="H44" s="207"/>
-      <c r="I44" s="208"/>
+      <c r="G44" s="204"/>
+      <c r="H44" s="204"/>
+      <c r="I44" s="205"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="167" t="s">
@@ -25550,18 +25584,18 @@
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="206" t="s">
+      <c r="A48" s="203" t="s">
         <v>1341</v>
       </c>
-      <c r="B48" s="207"/>
-      <c r="C48" s="207"/>
-      <c r="D48" s="208"/>
-      <c r="F48" s="206" t="s">
+      <c r="B48" s="204"/>
+      <c r="C48" s="204"/>
+      <c r="D48" s="205"/>
+      <c r="F48" s="203" t="s">
         <v>1341</v>
       </c>
-      <c r="G48" s="207"/>
-      <c r="H48" s="207"/>
-      <c r="I48" s="208"/>
+      <c r="G48" s="204"/>
+      <c r="H48" s="204"/>
+      <c r="I48" s="205"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="167" t="s">
@@ -25643,32 +25677,32 @@
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1"/>
     <row r="53" spans="1:9" ht="18">
-      <c r="A53" s="199" t="s">
+      <c r="A53" s="201" t="s">
         <v>1302</v>
       </c>
-      <c r="B53" s="205"/>
-      <c r="C53" s="205"/>
-      <c r="D53" s="200"/>
-      <c r="F53" s="199" t="s">
+      <c r="B53" s="206"/>
+      <c r="C53" s="206"/>
+      <c r="D53" s="202"/>
+      <c r="F53" s="201" t="s">
         <v>1302</v>
       </c>
-      <c r="G53" s="205"/>
-      <c r="H53" s="205"/>
-      <c r="I53" s="200"/>
+      <c r="G53" s="206"/>
+      <c r="H53" s="206"/>
+      <c r="I53" s="202"/>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="201" t="s">
+      <c r="A54" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="B54" s="209"/>
-      <c r="C54" s="209"/>
-      <c r="D54" s="202"/>
-      <c r="F54" s="201" t="s">
+      <c r="B54" s="207"/>
+      <c r="C54" s="207"/>
+      <c r="D54" s="200"/>
+      <c r="F54" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="G54" s="209"/>
-      <c r="H54" s="209"/>
-      <c r="I54" s="202"/>
+      <c r="G54" s="207"/>
+      <c r="H54" s="207"/>
+      <c r="I54" s="200"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="161" t="s">
@@ -25743,88 +25777,88 @@
       <c r="I58" s="162"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="201" t="s">
+      <c r="A59" s="199" t="s">
         <v>1310</v>
       </c>
-      <c r="B59" s="209"/>
-      <c r="C59" s="209"/>
-      <c r="D59" s="202"/>
-      <c r="F59" s="201" t="s">
+      <c r="B59" s="207"/>
+      <c r="C59" s="207"/>
+      <c r="D59" s="200"/>
+      <c r="F59" s="199" t="s">
         <v>1310</v>
       </c>
-      <c r="G59" s="209"/>
-      <c r="H59" s="209"/>
-      <c r="I59" s="202"/>
+      <c r="G59" s="207"/>
+      <c r="H59" s="207"/>
+      <c r="I59" s="200"/>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="210" t="s">
+      <c r="A60" s="208" t="s">
         <v>1311</v>
       </c>
-      <c r="B60" s="211"/>
-      <c r="C60" s="211"/>
-      <c r="D60" s="212"/>
-      <c r="F60" s="210" t="s">
+      <c r="B60" s="209"/>
+      <c r="C60" s="209"/>
+      <c r="D60" s="210"/>
+      <c r="F60" s="208" t="s">
         <v>1311</v>
       </c>
-      <c r="G60" s="211"/>
-      <c r="H60" s="211"/>
-      <c r="I60" s="212"/>
+      <c r="G60" s="209"/>
+      <c r="H60" s="209"/>
+      <c r="I60" s="210"/>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="201" t="s">
+      <c r="A61" s="199" t="s">
         <v>1312</v>
       </c>
-      <c r="B61" s="209"/>
-      <c r="C61" s="209"/>
-      <c r="D61" s="202"/>
-      <c r="F61" s="201" t="s">
+      <c r="B61" s="207"/>
+      <c r="C61" s="207"/>
+      <c r="D61" s="200"/>
+      <c r="F61" s="199" t="s">
         <v>1312</v>
       </c>
-      <c r="G61" s="209"/>
-      <c r="H61" s="209"/>
-      <c r="I61" s="202"/>
+      <c r="G61" s="207"/>
+      <c r="H61" s="207"/>
+      <c r="I61" s="200"/>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="210" t="s">
+      <c r="A62" s="208" t="s">
         <v>1313</v>
       </c>
-      <c r="B62" s="211"/>
-      <c r="C62" s="211"/>
-      <c r="D62" s="212"/>
-      <c r="F62" s="210" t="s">
+      <c r="B62" s="209"/>
+      <c r="C62" s="209"/>
+      <c r="D62" s="210"/>
+      <c r="F62" s="208" t="s">
         <v>1313</v>
       </c>
-      <c r="G62" s="211"/>
-      <c r="H62" s="211"/>
-      <c r="I62" s="212"/>
+      <c r="G62" s="209"/>
+      <c r="H62" s="209"/>
+      <c r="I62" s="210"/>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="201" t="s">
+      <c r="A63" s="199" t="s">
         <v>1314</v>
       </c>
-      <c r="B63" s="209"/>
-      <c r="C63" s="209"/>
-      <c r="D63" s="202"/>
-      <c r="F63" s="201" t="s">
+      <c r="B63" s="207"/>
+      <c r="C63" s="207"/>
+      <c r="D63" s="200"/>
+      <c r="F63" s="199" t="s">
         <v>1314</v>
       </c>
-      <c r="G63" s="209"/>
-      <c r="H63" s="209"/>
-      <c r="I63" s="202"/>
+      <c r="G63" s="207"/>
+      <c r="H63" s="207"/>
+      <c r="I63" s="200"/>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="206" t="s">
+      <c r="A64" s="203" t="s">
         <v>1315</v>
       </c>
-      <c r="B64" s="207"/>
-      <c r="C64" s="207"/>
-      <c r="D64" s="208"/>
-      <c r="F64" s="206" t="s">
+      <c r="B64" s="204"/>
+      <c r="C64" s="204"/>
+      <c r="D64" s="205"/>
+      <c r="F64" s="203" t="s">
         <v>1315</v>
       </c>
-      <c r="G64" s="207"/>
-      <c r="H64" s="207"/>
-      <c r="I64" s="208"/>
+      <c r="G64" s="204"/>
+      <c r="H64" s="204"/>
+      <c r="I64" s="205"/>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="167" t="s">
@@ -25959,18 +25993,18 @@
       <c r="I70" s="162"/>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="206" t="s">
+      <c r="A71" s="203" t="s">
         <v>1323</v>
       </c>
-      <c r="B71" s="207"/>
-      <c r="C71" s="207"/>
-      <c r="D71" s="208"/>
-      <c r="F71" s="206" t="s">
+      <c r="B71" s="204"/>
+      <c r="C71" s="204"/>
+      <c r="D71" s="205"/>
+      <c r="F71" s="203" t="s">
         <v>1323</v>
       </c>
-      <c r="G71" s="207"/>
-      <c r="H71" s="207"/>
-      <c r="I71" s="208"/>
+      <c r="G71" s="204"/>
+      <c r="H71" s="204"/>
+      <c r="I71" s="205"/>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="167" t="s">
@@ -26099,18 +26133,18 @@
       <c r="I78" s="162"/>
     </row>
     <row r="79" spans="1:9">
-      <c r="A79" s="206" t="s">
+      <c r="A79" s="203" t="s">
         <v>1329</v>
       </c>
-      <c r="B79" s="207"/>
-      <c r="C79" s="207"/>
-      <c r="D79" s="208"/>
-      <c r="F79" s="206" t="s">
+      <c r="B79" s="204"/>
+      <c r="C79" s="204"/>
+      <c r="D79" s="205"/>
+      <c r="F79" s="203" t="s">
         <v>1329</v>
       </c>
-      <c r="G79" s="207"/>
-      <c r="H79" s="207"/>
-      <c r="I79" s="208"/>
+      <c r="G79" s="204"/>
+      <c r="H79" s="204"/>
+      <c r="I79" s="205"/>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="167" t="s">
@@ -26191,18 +26225,18 @@
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="206" t="s">
+      <c r="A83" s="203" t="s">
         <v>1341</v>
       </c>
-      <c r="B83" s="207"/>
-      <c r="C83" s="207"/>
-      <c r="D83" s="208"/>
-      <c r="F83" s="206" t="s">
+      <c r="B83" s="204"/>
+      <c r="C83" s="204"/>
+      <c r="D83" s="205"/>
+      <c r="F83" s="203" t="s">
         <v>1341</v>
       </c>
-      <c r="G83" s="207"/>
-      <c r="H83" s="207"/>
-      <c r="I83" s="208"/>
+      <c r="G83" s="204"/>
+      <c r="H83" s="204"/>
+      <c r="I83" s="205"/>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="167" t="s">
@@ -26310,32 +26344,32 @@
     </row>
     <row r="89" spans="1:9" ht="15" thickBot="1"/>
     <row r="90" spans="1:9" ht="18">
-      <c r="A90" s="199" t="s">
+      <c r="A90" s="201" t="s">
         <v>1302</v>
       </c>
-      <c r="B90" s="205"/>
-      <c r="C90" s="205"/>
-      <c r="D90" s="200"/>
-      <c r="F90" s="199" t="s">
+      <c r="B90" s="206"/>
+      <c r="C90" s="206"/>
+      <c r="D90" s="202"/>
+      <c r="F90" s="201" t="s">
         <v>1302</v>
       </c>
-      <c r="G90" s="205"/>
-      <c r="H90" s="205"/>
-      <c r="I90" s="200"/>
+      <c r="G90" s="206"/>
+      <c r="H90" s="206"/>
+      <c r="I90" s="202"/>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="201" t="s">
+      <c r="A91" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="B91" s="209"/>
-      <c r="C91" s="209"/>
-      <c r="D91" s="202"/>
-      <c r="F91" s="201" t="s">
+      <c r="B91" s="207"/>
+      <c r="C91" s="207"/>
+      <c r="D91" s="200"/>
+      <c r="F91" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="G91" s="209"/>
-      <c r="H91" s="209"/>
-      <c r="I91" s="202"/>
+      <c r="G91" s="207"/>
+      <c r="H91" s="207"/>
+      <c r="I91" s="200"/>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="161" t="s">
@@ -26410,88 +26444,88 @@
       <c r="I95" s="162"/>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="201" t="s">
+      <c r="A96" s="199" t="s">
         <v>1310</v>
       </c>
-      <c r="B96" s="209"/>
-      <c r="C96" s="209"/>
-      <c r="D96" s="202"/>
-      <c r="F96" s="201" t="s">
+      <c r="B96" s="207"/>
+      <c r="C96" s="207"/>
+      <c r="D96" s="200"/>
+      <c r="F96" s="199" t="s">
         <v>1310</v>
       </c>
-      <c r="G96" s="209"/>
-      <c r="H96" s="209"/>
-      <c r="I96" s="202"/>
+      <c r="G96" s="207"/>
+      <c r="H96" s="207"/>
+      <c r="I96" s="200"/>
     </row>
     <row r="97" spans="1:9">
-      <c r="A97" s="210" t="s">
+      <c r="A97" s="208" t="s">
         <v>1311</v>
       </c>
-      <c r="B97" s="211"/>
-      <c r="C97" s="211"/>
-      <c r="D97" s="212"/>
-      <c r="F97" s="210" t="s">
+      <c r="B97" s="209"/>
+      <c r="C97" s="209"/>
+      <c r="D97" s="210"/>
+      <c r="F97" s="208" t="s">
         <v>1311</v>
       </c>
-      <c r="G97" s="211"/>
-      <c r="H97" s="211"/>
-      <c r="I97" s="212"/>
+      <c r="G97" s="209"/>
+      <c r="H97" s="209"/>
+      <c r="I97" s="210"/>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="201" t="s">
+      <c r="A98" s="199" t="s">
         <v>1312</v>
       </c>
-      <c r="B98" s="209"/>
-      <c r="C98" s="209"/>
-      <c r="D98" s="202"/>
-      <c r="F98" s="201" t="s">
+      <c r="B98" s="207"/>
+      <c r="C98" s="207"/>
+      <c r="D98" s="200"/>
+      <c r="F98" s="199" t="s">
         <v>1312</v>
       </c>
-      <c r="G98" s="209"/>
-      <c r="H98" s="209"/>
-      <c r="I98" s="202"/>
+      <c r="G98" s="207"/>
+      <c r="H98" s="207"/>
+      <c r="I98" s="200"/>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="210" t="s">
+      <c r="A99" s="208" t="s">
         <v>1313</v>
       </c>
-      <c r="B99" s="211"/>
-      <c r="C99" s="211"/>
-      <c r="D99" s="212"/>
-      <c r="F99" s="210" t="s">
+      <c r="B99" s="209"/>
+      <c r="C99" s="209"/>
+      <c r="D99" s="210"/>
+      <c r="F99" s="208" t="s">
         <v>1313</v>
       </c>
-      <c r="G99" s="211"/>
-      <c r="H99" s="211"/>
-      <c r="I99" s="212"/>
+      <c r="G99" s="209"/>
+      <c r="H99" s="209"/>
+      <c r="I99" s="210"/>
     </row>
     <row r="100" spans="1:9">
-      <c r="A100" s="201" t="s">
+      <c r="A100" s="199" t="s">
         <v>1314</v>
       </c>
-      <c r="B100" s="209"/>
-      <c r="C100" s="209"/>
-      <c r="D100" s="202"/>
-      <c r="F100" s="201" t="s">
+      <c r="B100" s="207"/>
+      <c r="C100" s="207"/>
+      <c r="D100" s="200"/>
+      <c r="F100" s="199" t="s">
         <v>1314</v>
       </c>
-      <c r="G100" s="209"/>
-      <c r="H100" s="209"/>
-      <c r="I100" s="202"/>
+      <c r="G100" s="207"/>
+      <c r="H100" s="207"/>
+      <c r="I100" s="200"/>
     </row>
     <row r="101" spans="1:9">
-      <c r="A101" s="206" t="s">
+      <c r="A101" s="203" t="s">
         <v>1315</v>
       </c>
-      <c r="B101" s="207"/>
-      <c r="C101" s="207"/>
-      <c r="D101" s="208"/>
-      <c r="F101" s="206" t="s">
+      <c r="B101" s="204"/>
+      <c r="C101" s="204"/>
+      <c r="D101" s="205"/>
+      <c r="F101" s="203" t="s">
         <v>1315</v>
       </c>
-      <c r="G101" s="207"/>
-      <c r="H101" s="207"/>
-      <c r="I101" s="208"/>
+      <c r="G101" s="204"/>
+      <c r="H101" s="204"/>
+      <c r="I101" s="205"/>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" s="167" t="s">
@@ -26626,18 +26660,18 @@
       <c r="I107" s="162"/>
     </row>
     <row r="108" spans="1:9">
-      <c r="A108" s="206" t="s">
+      <c r="A108" s="203" t="s">
         <v>1323</v>
       </c>
-      <c r="B108" s="207"/>
-      <c r="C108" s="207"/>
-      <c r="D108" s="208"/>
-      <c r="F108" s="206" t="s">
+      <c r="B108" s="204"/>
+      <c r="C108" s="204"/>
+      <c r="D108" s="205"/>
+      <c r="F108" s="203" t="s">
         <v>1323</v>
       </c>
-      <c r="G108" s="207"/>
-      <c r="H108" s="207"/>
-      <c r="I108" s="208"/>
+      <c r="G108" s="204"/>
+      <c r="H108" s="204"/>
+      <c r="I108" s="205"/>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" s="167" t="s">
@@ -26766,18 +26800,18 @@
       <c r="I115" s="162"/>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="206" t="s">
+      <c r="A116" s="203" t="s">
         <v>1329</v>
       </c>
-      <c r="B116" s="207"/>
-      <c r="C116" s="207"/>
-      <c r="D116" s="208"/>
-      <c r="F116" s="206" t="s">
+      <c r="B116" s="204"/>
+      <c r="C116" s="204"/>
+      <c r="D116" s="205"/>
+      <c r="F116" s="203" t="s">
         <v>1329</v>
       </c>
-      <c r="G116" s="207"/>
-      <c r="H116" s="207"/>
-      <c r="I116" s="208"/>
+      <c r="G116" s="204"/>
+      <c r="H116" s="204"/>
+      <c r="I116" s="205"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" s="167" t="s">
@@ -26858,18 +26892,18 @@
       </c>
     </row>
     <row r="120" spans="1:9">
-      <c r="A120" s="206" t="s">
+      <c r="A120" s="203" t="s">
         <v>1341</v>
       </c>
-      <c r="B120" s="207"/>
-      <c r="C120" s="207"/>
-      <c r="D120" s="208"/>
-      <c r="F120" s="206" t="s">
+      <c r="B120" s="204"/>
+      <c r="C120" s="204"/>
+      <c r="D120" s="205"/>
+      <c r="F120" s="203" t="s">
         <v>1341</v>
       </c>
-      <c r="G120" s="207"/>
-      <c r="H120" s="207"/>
-      <c r="I120" s="208"/>
+      <c r="G120" s="204"/>
+      <c r="H120" s="204"/>
+      <c r="I120" s="205"/>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" s="167" t="s">
@@ -26977,32 +27011,32 @@
     </row>
     <row r="126" spans="1:9" ht="15" thickBot="1"/>
     <row r="127" spans="1:9" ht="18">
-      <c r="A127" s="199" t="s">
+      <c r="A127" s="201" t="s">
         <v>1302</v>
       </c>
-      <c r="B127" s="205"/>
-      <c r="C127" s="205"/>
-      <c r="D127" s="200"/>
-      <c r="F127" s="199" t="s">
+      <c r="B127" s="206"/>
+      <c r="C127" s="206"/>
+      <c r="D127" s="202"/>
+      <c r="F127" s="201" t="s">
         <v>1302</v>
       </c>
-      <c r="G127" s="205"/>
-      <c r="H127" s="205"/>
-      <c r="I127" s="200"/>
+      <c r="G127" s="206"/>
+      <c r="H127" s="206"/>
+      <c r="I127" s="202"/>
     </row>
     <row r="128" spans="1:9">
-      <c r="A128" s="201" t="s">
+      <c r="A128" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="B128" s="209"/>
-      <c r="C128" s="209"/>
-      <c r="D128" s="202"/>
-      <c r="F128" s="201" t="s">
+      <c r="B128" s="207"/>
+      <c r="C128" s="207"/>
+      <c r="D128" s="200"/>
+      <c r="F128" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="G128" s="209"/>
-      <c r="H128" s="209"/>
-      <c r="I128" s="202"/>
+      <c r="G128" s="207"/>
+      <c r="H128" s="207"/>
+      <c r="I128" s="200"/>
     </row>
     <row r="129" spans="1:9">
       <c r="A129" s="161" t="s">
@@ -27077,88 +27111,88 @@
       <c r="I132" s="162"/>
     </row>
     <row r="133" spans="1:9">
-      <c r="A133" s="201" t="s">
+      <c r="A133" s="199" t="s">
         <v>1310</v>
       </c>
-      <c r="B133" s="209"/>
-      <c r="C133" s="209"/>
-      <c r="D133" s="202"/>
-      <c r="F133" s="201" t="s">
+      <c r="B133" s="207"/>
+      <c r="C133" s="207"/>
+      <c r="D133" s="200"/>
+      <c r="F133" s="199" t="s">
         <v>1310</v>
       </c>
-      <c r="G133" s="209"/>
-      <c r="H133" s="209"/>
-      <c r="I133" s="202"/>
+      <c r="G133" s="207"/>
+      <c r="H133" s="207"/>
+      <c r="I133" s="200"/>
     </row>
     <row r="134" spans="1:9">
-      <c r="A134" s="210" t="s">
+      <c r="A134" s="208" t="s">
         <v>1311</v>
       </c>
-      <c r="B134" s="211"/>
-      <c r="C134" s="211"/>
-      <c r="D134" s="212"/>
-      <c r="F134" s="210" t="s">
+      <c r="B134" s="209"/>
+      <c r="C134" s="209"/>
+      <c r="D134" s="210"/>
+      <c r="F134" s="208" t="s">
         <v>1311</v>
       </c>
-      <c r="G134" s="211"/>
-      <c r="H134" s="211"/>
-      <c r="I134" s="212"/>
+      <c r="G134" s="209"/>
+      <c r="H134" s="209"/>
+      <c r="I134" s="210"/>
     </row>
     <row r="135" spans="1:9">
-      <c r="A135" s="201" t="s">
+      <c r="A135" s="199" t="s">
         <v>1312</v>
       </c>
-      <c r="B135" s="209"/>
-      <c r="C135" s="209"/>
-      <c r="D135" s="202"/>
-      <c r="F135" s="201" t="s">
+      <c r="B135" s="207"/>
+      <c r="C135" s="207"/>
+      <c r="D135" s="200"/>
+      <c r="F135" s="199" t="s">
         <v>1312</v>
       </c>
-      <c r="G135" s="209"/>
-      <c r="H135" s="209"/>
-      <c r="I135" s="202"/>
+      <c r="G135" s="207"/>
+      <c r="H135" s="207"/>
+      <c r="I135" s="200"/>
     </row>
     <row r="136" spans="1:9">
-      <c r="A136" s="210" t="s">
+      <c r="A136" s="208" t="s">
         <v>1313</v>
       </c>
-      <c r="B136" s="211"/>
-      <c r="C136" s="211"/>
-      <c r="D136" s="212"/>
-      <c r="F136" s="210" t="s">
+      <c r="B136" s="209"/>
+      <c r="C136" s="209"/>
+      <c r="D136" s="210"/>
+      <c r="F136" s="208" t="s">
         <v>1313</v>
       </c>
-      <c r="G136" s="211"/>
-      <c r="H136" s="211"/>
-      <c r="I136" s="212"/>
+      <c r="G136" s="209"/>
+      <c r="H136" s="209"/>
+      <c r="I136" s="210"/>
     </row>
     <row r="137" spans="1:9">
-      <c r="A137" s="201" t="s">
+      <c r="A137" s="199" t="s">
         <v>1314</v>
       </c>
-      <c r="B137" s="209"/>
-      <c r="C137" s="209"/>
-      <c r="D137" s="202"/>
-      <c r="F137" s="201" t="s">
+      <c r="B137" s="207"/>
+      <c r="C137" s="207"/>
+      <c r="D137" s="200"/>
+      <c r="F137" s="199" t="s">
         <v>1314</v>
       </c>
-      <c r="G137" s="209"/>
-      <c r="H137" s="209"/>
-      <c r="I137" s="202"/>
+      <c r="G137" s="207"/>
+      <c r="H137" s="207"/>
+      <c r="I137" s="200"/>
     </row>
     <row r="138" spans="1:9">
-      <c r="A138" s="206" t="s">
+      <c r="A138" s="203" t="s">
         <v>1315</v>
       </c>
-      <c r="B138" s="207"/>
-      <c r="C138" s="207"/>
-      <c r="D138" s="208"/>
-      <c r="F138" s="206" t="s">
+      <c r="B138" s="204"/>
+      <c r="C138" s="204"/>
+      <c r="D138" s="205"/>
+      <c r="F138" s="203" t="s">
         <v>1315</v>
       </c>
-      <c r="G138" s="207"/>
-      <c r="H138" s="207"/>
-      <c r="I138" s="208"/>
+      <c r="G138" s="204"/>
+      <c r="H138" s="204"/>
+      <c r="I138" s="205"/>
     </row>
     <row r="139" spans="1:9">
       <c r="A139" s="167" t="s">
@@ -27293,18 +27327,18 @@
       <c r="I144" s="162"/>
     </row>
     <row r="145" spans="1:9">
-      <c r="A145" s="206" t="s">
+      <c r="A145" s="203" t="s">
         <v>1323</v>
       </c>
-      <c r="B145" s="207"/>
-      <c r="C145" s="207"/>
-      <c r="D145" s="208"/>
-      <c r="F145" s="206" t="s">
+      <c r="B145" s="204"/>
+      <c r="C145" s="204"/>
+      <c r="D145" s="205"/>
+      <c r="F145" s="203" t="s">
         <v>1323</v>
       </c>
-      <c r="G145" s="207"/>
-      <c r="H145" s="207"/>
-      <c r="I145" s="208"/>
+      <c r="G145" s="204"/>
+      <c r="H145" s="204"/>
+      <c r="I145" s="205"/>
     </row>
     <row r="146" spans="1:9">
       <c r="A146" s="167" t="s">
@@ -27433,18 +27467,18 @@
       <c r="I152" s="162"/>
     </row>
     <row r="153" spans="1:9">
-      <c r="A153" s="206" t="s">
+      <c r="A153" s="203" t="s">
         <v>1329</v>
       </c>
-      <c r="B153" s="207"/>
-      <c r="C153" s="207"/>
-      <c r="D153" s="208"/>
-      <c r="F153" s="206" t="s">
+      <c r="B153" s="204"/>
+      <c r="C153" s="204"/>
+      <c r="D153" s="205"/>
+      <c r="F153" s="203" t="s">
         <v>1329</v>
       </c>
-      <c r="G153" s="207"/>
-      <c r="H153" s="207"/>
-      <c r="I153" s="208"/>
+      <c r="G153" s="204"/>
+      <c r="H153" s="204"/>
+      <c r="I153" s="205"/>
     </row>
     <row r="154" spans="1:9">
       <c r="A154" s="167" t="s">
@@ -27525,18 +27559,18 @@
       </c>
     </row>
     <row r="157" spans="1:9">
-      <c r="A157" s="206" t="s">
+      <c r="A157" s="203" t="s">
         <v>1341</v>
       </c>
-      <c r="B157" s="207"/>
-      <c r="C157" s="207"/>
-      <c r="D157" s="208"/>
-      <c r="F157" s="206" t="s">
+      <c r="B157" s="204"/>
+      <c r="C157" s="204"/>
+      <c r="D157" s="205"/>
+      <c r="F157" s="203" t="s">
         <v>1341</v>
       </c>
-      <c r="G157" s="207"/>
-      <c r="H157" s="207"/>
-      <c r="I157" s="208"/>
+      <c r="G157" s="204"/>
+      <c r="H157" s="204"/>
+      <c r="I157" s="205"/>
     </row>
     <row r="158" spans="1:9">
       <c r="A158" s="167" t="s">
@@ -27618,24 +27652,24 @@
     </row>
     <row r="164" spans="1:7" ht="15" thickBot="1"/>
     <row r="165" spans="1:7" ht="18">
-      <c r="A165" s="199" t="s">
+      <c r="A165" s="201" t="s">
         <v>1423</v>
       </c>
-      <c r="B165" s="200"/>
-      <c r="F165" s="199" t="s">
+      <c r="B165" s="202"/>
+      <c r="F165" s="201" t="s">
         <v>1423</v>
       </c>
-      <c r="G165" s="200"/>
+      <c r="G165" s="202"/>
     </row>
     <row r="166" spans="1:7">
-      <c r="A166" s="201" t="s">
+      <c r="A166" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="B166" s="202"/>
-      <c r="F166" s="201" t="s">
+      <c r="B166" s="200"/>
+      <c r="F166" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="G166" s="202"/>
+      <c r="G166" s="200"/>
     </row>
     <row r="167" spans="1:7">
       <c r="A167" s="161" t="s">
@@ -27666,14 +27700,14 @@
       </c>
     </row>
     <row r="169" spans="1:7">
-      <c r="A169" s="201" t="s">
+      <c r="A169" s="199" t="s">
         <v>1287</v>
       </c>
-      <c r="B169" s="202"/>
-      <c r="F169" s="201" t="s">
+      <c r="B169" s="200"/>
+      <c r="F169" s="199" t="s">
         <v>1287</v>
       </c>
-      <c r="G169" s="202"/>
+      <c r="G169" s="200"/>
     </row>
     <row r="170" spans="1:7">
       <c r="A170" s="161" t="s">
@@ -27704,14 +27738,14 @@
       </c>
     </row>
     <row r="172" spans="1:7">
-      <c r="A172" s="201" t="s">
+      <c r="A172" s="199" t="s">
         <v>1428</v>
       </c>
-      <c r="B172" s="202"/>
-      <c r="F172" s="201" t="s">
+      <c r="B172" s="200"/>
+      <c r="F172" s="199" t="s">
         <v>1428</v>
       </c>
-      <c r="G172" s="202"/>
+      <c r="G172" s="200"/>
     </row>
     <row r="173" spans="1:7">
       <c r="A173" s="161" t="s">
@@ -27742,14 +27776,14 @@
       </c>
     </row>
     <row r="175" spans="1:7">
-      <c r="A175" s="201" t="s">
+      <c r="A175" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="B175" s="202"/>
-      <c r="F175" s="201" t="s">
+      <c r="B175" s="200"/>
+      <c r="F175" s="199" t="s">
         <v>1432</v>
       </c>
-      <c r="G175" s="202"/>
+      <c r="G175" s="200"/>
     </row>
     <row r="176" spans="1:7">
       <c r="A176" s="161" t="s">
@@ -27809,16 +27843,16 @@
     </row>
     <row r="181" spans="1:7" ht="15" thickBot="1"/>
     <row r="182" spans="1:7" ht="18">
-      <c r="A182" s="199" t="s">
+      <c r="A182" s="201" t="s">
         <v>1434</v>
       </c>
-      <c r="B182" s="200"/>
+      <c r="B182" s="202"/>
     </row>
     <row r="183" spans="1:7">
-      <c r="A183" s="201" t="s">
+      <c r="A183" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="B183" s="202"/>
+      <c r="B183" s="200"/>
     </row>
     <row r="184" spans="1:7">
       <c r="A184" s="161" t="s">
@@ -27837,10 +27871,10 @@
       </c>
     </row>
     <row r="186" spans="1:7">
-      <c r="A186" s="201" t="s">
+      <c r="A186" s="199" t="s">
         <v>1436</v>
       </c>
-      <c r="B186" s="202"/>
+      <c r="B186" s="200"/>
     </row>
     <row r="187" spans="1:7">
       <c r="A187" s="161" t="s">
@@ -27875,10 +27909,10 @@
       </c>
     </row>
     <row r="191" spans="1:7">
-      <c r="A191" s="201" t="s">
+      <c r="A191" s="199" t="s">
         <v>1443</v>
       </c>
-      <c r="B191" s="202"/>
+      <c r="B191" s="200"/>
     </row>
     <row r="192" spans="1:7">
       <c r="A192" s="161" t="s">
@@ -27934,24 +27968,24 @@
     </row>
     <row r="199" spans="1:7" ht="15" thickBot="1"/>
     <row r="200" spans="1:7" ht="18">
-      <c r="A200" s="199" t="s">
+      <c r="A200" s="201" t="s">
         <v>1448</v>
       </c>
-      <c r="B200" s="200"/>
-      <c r="F200" s="199" t="s">
+      <c r="B200" s="202"/>
+      <c r="F200" s="201" t="s">
         <v>1448</v>
       </c>
-      <c r="G200" s="200"/>
+      <c r="G200" s="202"/>
     </row>
     <row r="201" spans="1:7">
-      <c r="A201" s="201" t="s">
+      <c r="A201" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="B201" s="202"/>
-      <c r="F201" s="201" t="s">
+      <c r="B201" s="200"/>
+      <c r="F201" s="199" t="s">
         <v>1281</v>
       </c>
-      <c r="G201" s="202"/>
+      <c r="G201" s="200"/>
     </row>
     <row r="202" spans="1:7">
       <c r="A202" s="161" t="s">
@@ -27982,77 +28016,67 @@
       </c>
     </row>
     <row r="204" spans="1:7">
-      <c r="A204" s="201" t="s">
+      <c r="A204" s="199" t="s">
         <v>1453</v>
       </c>
-      <c r="B204" s="202"/>
-      <c r="F204" s="201" t="s">
+      <c r="B204" s="200"/>
+      <c r="F204" s="199" t="s">
         <v>1453</v>
       </c>
-      <c r="G204" s="202"/>
+      <c r="G204" s="200"/>
     </row>
     <row r="205" spans="1:7" ht="15" thickBot="1">
-      <c r="A205" s="203" t="s">
+      <c r="A205" s="211" t="s">
         <v>1454</v>
       </c>
-      <c r="B205" s="204"/>
-      <c r="F205" s="203" t="s">
+      <c r="B205" s="212"/>
+      <c r="F205" s="211" t="s">
         <v>1454</v>
       </c>
-      <c r="G205" s="204"/>
+      <c r="G205" s="212"/>
     </row>
   </sheetData>
   <mergeCells count="114">
-    <mergeCell ref="A191:B191"/>
-    <mergeCell ref="A182:B182"/>
-    <mergeCell ref="A183:B183"/>
-    <mergeCell ref="A186:B186"/>
-    <mergeCell ref="F165:G165"/>
-    <mergeCell ref="F166:G166"/>
-    <mergeCell ref="F169:G169"/>
-    <mergeCell ref="F172:G172"/>
-    <mergeCell ref="F175:G175"/>
-    <mergeCell ref="A165:B165"/>
-    <mergeCell ref="A166:B166"/>
-    <mergeCell ref="A169:B169"/>
-    <mergeCell ref="A172:B172"/>
-    <mergeCell ref="A175:B175"/>
-    <mergeCell ref="F157:I157"/>
-    <mergeCell ref="F120:I120"/>
-    <mergeCell ref="F127:I127"/>
-    <mergeCell ref="F128:I128"/>
-    <mergeCell ref="F133:I133"/>
-    <mergeCell ref="F134:I134"/>
-    <mergeCell ref="F135:I135"/>
-    <mergeCell ref="F136:I136"/>
-    <mergeCell ref="F137:I137"/>
-    <mergeCell ref="F138:I138"/>
-    <mergeCell ref="F145:I145"/>
-    <mergeCell ref="F153:I153"/>
-    <mergeCell ref="F116:I116"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="F83:I83"/>
-    <mergeCell ref="F90:I90"/>
-    <mergeCell ref="F91:I91"/>
-    <mergeCell ref="F96:I96"/>
-    <mergeCell ref="F97:I97"/>
-    <mergeCell ref="F98:I98"/>
-    <mergeCell ref="F99:I99"/>
-    <mergeCell ref="F100:I100"/>
-    <mergeCell ref="F101:I101"/>
-    <mergeCell ref="F108:I108"/>
-    <mergeCell ref="F71:I71"/>
-    <mergeCell ref="F36:I36"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="F62:I62"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="A200:B200"/>
+    <mergeCell ref="A201:B201"/>
+    <mergeCell ref="A204:B204"/>
+    <mergeCell ref="A205:B205"/>
+    <mergeCell ref="F200:G200"/>
+    <mergeCell ref="F201:G201"/>
+    <mergeCell ref="F204:G204"/>
+    <mergeCell ref="F205:G205"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A53:D53"/>
+    <mergeCell ref="A44:D44"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A54:D54"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A62:D62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A90:D90"/>
     <mergeCell ref="A153:D153"/>
     <mergeCell ref="A157:D157"/>
     <mergeCell ref="F18:I18"/>
@@ -28077,46 +28101,56 @@
     <mergeCell ref="A100:D100"/>
     <mergeCell ref="A101:D101"/>
     <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A128:D128"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A62:D62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="A200:B200"/>
-    <mergeCell ref="A201:B201"/>
-    <mergeCell ref="A204:B204"/>
-    <mergeCell ref="A205:B205"/>
-    <mergeCell ref="F200:G200"/>
-    <mergeCell ref="F201:G201"/>
-    <mergeCell ref="F204:G204"/>
-    <mergeCell ref="F205:G205"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A53:D53"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="F71:I71"/>
+    <mergeCell ref="F36:I36"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="F116:I116"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="F83:I83"/>
+    <mergeCell ref="F90:I90"/>
+    <mergeCell ref="F91:I91"/>
+    <mergeCell ref="F96:I96"/>
+    <mergeCell ref="F97:I97"/>
+    <mergeCell ref="F98:I98"/>
+    <mergeCell ref="F99:I99"/>
+    <mergeCell ref="F100:I100"/>
+    <mergeCell ref="F101:I101"/>
+    <mergeCell ref="F108:I108"/>
+    <mergeCell ref="F157:I157"/>
+    <mergeCell ref="F120:I120"/>
+    <mergeCell ref="F127:I127"/>
+    <mergeCell ref="F128:I128"/>
+    <mergeCell ref="F133:I133"/>
+    <mergeCell ref="F134:I134"/>
+    <mergeCell ref="F135:I135"/>
+    <mergeCell ref="F136:I136"/>
+    <mergeCell ref="F137:I137"/>
+    <mergeCell ref="F138:I138"/>
+    <mergeCell ref="F145:I145"/>
+    <mergeCell ref="F153:I153"/>
+    <mergeCell ref="A191:B191"/>
+    <mergeCell ref="A182:B182"/>
+    <mergeCell ref="A183:B183"/>
+    <mergeCell ref="A186:B186"/>
+    <mergeCell ref="F165:G165"/>
+    <mergeCell ref="F166:G166"/>
+    <mergeCell ref="F169:G169"/>
+    <mergeCell ref="F172:G172"/>
+    <mergeCell ref="F175:G175"/>
+    <mergeCell ref="A165:B165"/>
+    <mergeCell ref="A166:B166"/>
+    <mergeCell ref="A169:B169"/>
+    <mergeCell ref="A172:B172"/>
+    <mergeCell ref="A175:B175"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -40520,6 +40554,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100C297A53C74A1D94EA9911408ECAC2CE1" ma:contentTypeVersion="9" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="29fe4b809f0fa0a45b06b6d73cb8b062">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="eaf262ef-7826-430c-9070-0dd2e6d0c7a3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a6a8143ca2b5c1326281a6d33e5e77d" ns2:_="">
     <xsd:import namespace="eaf262ef-7826-430c-9070-0dd2e6d0c7a3"/>
@@ -40695,15 +40738,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C87939E5-2E1D-451A-AA58-3A58F63DCD26}">
   <ds:schemaRefs>
@@ -40721,6 +40755,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6A03F3-6EBC-493D-9331-FC3669ADBF91}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7F8EE32C-953B-475C-B1D1-EEEF2FE07B19}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40736,12 +40778,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6A03F3-6EBC-493D-9331-FC3669ADBF91}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixes #23, 2x new excel, readme changed
</commit_message>
<xml_diff>
--- a/feste-script/wip_checkliste_gesamt.xlsx
+++ b/feste-script/wip_checkliste_gesamt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://concat-my.sharepoint.com/personal/oliver_antwerpen_concat_de/Documents/Kunden/ITSG/DiGeN/posh/xls-wip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="101_{BAA6B38C-8C0A-40AE-8FC2-2C92A8B77B8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1216B8F-58C8-4AA5-9F09-8D4D23BF69A0}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="101_{BAA6B38C-8C0A-40AE-8FC2-2C92A8B77B8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{75CCB52D-5082-4281-810A-EAD5E5B04169}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="1095" windowWidth="25440" windowHeight="15390" tabRatio="870" firstSheet="14" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="870" firstSheet="14" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Changelog" sheetId="26" r:id="rId1"/>
@@ -11248,21 +11248,21 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{88638CF4-4B51-404C-8ECA-437A98720BB3}" name="Tabelle18" displayName="Tabelle18" ref="A1:L22" totalsRowShown="0" headerRowDxfId="174" dataDxfId="173">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{88638CF4-4B51-404C-8ECA-437A98720BB3}" name="Tabelle18" displayName="Tabelle18" ref="A1:L22" totalsRowShown="0" headerRowDxfId="161" dataDxfId="160">
   <autoFilter ref="A1:L22" xr:uid="{C8ED7277-4C2A-4869-8F71-893322FE1EB5}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{32C158CD-E5C1-412C-ABEA-31B90FA6B0A1}" name="Zone" dataDxfId="172"/>
-    <tableColumn id="2" xr3:uid="{DD857513-5BB8-4A19-A194-7BE5C5F37A1A}" name="Name" dataDxfId="171"/>
-    <tableColumn id="3" xr3:uid="{DE020B8F-E6A1-4D23-8127-7275F9462DD3}" name="Type" dataDxfId="170"/>
-    <tableColumn id="4" xr3:uid="{2C53B1A8-030C-4B38-A4E7-2E018389656A}" name="SubnetID" dataDxfId="169"/>
-    <tableColumn id="5" xr3:uid="{C7E4B0B1-3549-4510-9B57-5223172FA28A}" name="SubnetMask" dataDxfId="168"/>
-    <tableColumn id="6" xr3:uid="{8A385309-2507-47B6-82B5-C0E2CBE39764}" name="Gateway" dataDxfId="167"/>
-    <tableColumn id="7" xr3:uid="{09E71725-F923-4B72-B9DD-5B3B364574C4}" name="Domain" dataDxfId="166"/>
-    <tableColumn id="8" xr3:uid="{96D404E1-7F74-4453-A0DB-60FF50E3D812}" name="DnsServer1" dataDxfId="165"/>
-    <tableColumn id="12" xr3:uid="{F3010178-84F9-4A15-9AD7-01380702506A}" name="DnsServer2" dataDxfId="164"/>
-    <tableColumn id="11" xr3:uid="{211E2654-FDFA-48B9-A2B6-7AB540F65AE4}" name="DnsServer3" dataDxfId="163"/>
-    <tableColumn id="9" xr3:uid="{4D5427C1-341C-4D2D-ADE4-9B2640B412A6}" name="RangeStart" dataDxfId="162"/>
-    <tableColumn id="10" xr3:uid="{6FE1C019-96E8-4C58-B4C7-CA4EEA6C76B5}" name="RangeEnd" dataDxfId="161"/>
+    <tableColumn id="1" xr3:uid="{32C158CD-E5C1-412C-ABEA-31B90FA6B0A1}" name="Zone" dataDxfId="159"/>
+    <tableColumn id="2" xr3:uid="{DD857513-5BB8-4A19-A194-7BE5C5F37A1A}" name="Name" dataDxfId="158"/>
+    <tableColumn id="3" xr3:uid="{DE020B8F-E6A1-4D23-8127-7275F9462DD3}" name="Type" dataDxfId="157"/>
+    <tableColumn id="4" xr3:uid="{2C53B1A8-030C-4B38-A4E7-2E018389656A}" name="SubnetID" dataDxfId="156"/>
+    <tableColumn id="5" xr3:uid="{C7E4B0B1-3549-4510-9B57-5223172FA28A}" name="SubnetMask" dataDxfId="155"/>
+    <tableColumn id="6" xr3:uid="{8A385309-2507-47B6-82B5-C0E2CBE39764}" name="Gateway" dataDxfId="154"/>
+    <tableColumn id="7" xr3:uid="{09E71725-F923-4B72-B9DD-5B3B364574C4}" name="Domain" dataDxfId="153"/>
+    <tableColumn id="8" xr3:uid="{96D404E1-7F74-4453-A0DB-60FF50E3D812}" name="DnsServer1" dataDxfId="152"/>
+    <tableColumn id="12" xr3:uid="{F3010178-84F9-4A15-9AD7-01380702506A}" name="DnsServer2" dataDxfId="151"/>
+    <tableColumn id="11" xr3:uid="{211E2654-FDFA-48B9-A2B6-7AB540F65AE4}" name="DnsServer3" dataDxfId="150"/>
+    <tableColumn id="9" xr3:uid="{4D5427C1-341C-4D2D-ADE4-9B2640B412A6}" name="RangeStart" dataDxfId="149"/>
+    <tableColumn id="10" xr3:uid="{6FE1C019-96E8-4C58-B4C7-CA4EEA6C76B5}" name="RangeEnd" dataDxfId="148"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11580,20 +11580,20 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{926181DA-CBAF-4928-B5F3-0E1A0777033E}" name="Tabelle6" displayName="Tabelle6" ref="B1:L14" totalsRowShown="0" headerRowDxfId="160" dataDxfId="159">
-  <autoFilter ref="B1:L14" xr:uid="{7766A357-26C6-4690-9C18-F7F16C78F028}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{926181DA-CBAF-4928-B5F3-0E1A0777033E}" name="Tabelle6" displayName="Tabelle6" ref="B1:L15" totalsRowShown="0" headerRowDxfId="174" dataDxfId="173">
+  <autoFilter ref="B1:L15" xr:uid="{7766A357-26C6-4690-9C18-F7F16C78F028}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{C9F95E78-00F2-4748-9AB8-00A9D57E226E}" name="Name" dataDxfId="158"/>
-    <tableColumn id="2" xr3:uid="{851B9CAB-3BBD-4E47-A479-93E1A6BB9555}" name="Purpose" dataDxfId="157"/>
-    <tableColumn id="3" xr3:uid="{A094AA9D-9339-475A-8F8A-F754CEB9212E}" name="Type" dataDxfId="156"/>
-    <tableColumn id="4" xr3:uid="{EA1F4E56-4974-4FF2-85B3-5E643B75708A}" name="VlanID" dataDxfId="155"/>
-    <tableColumn id="5" xr3:uid="{78D39E12-D3F8-4781-8503-8CC2A850C2F1}" name="IPv4Subnet" dataDxfId="154"/>
-    <tableColumn id="6" xr3:uid="{9DF7F43F-8572-4BCB-93D1-4C30EA4AD9B8}" name="Smartlink" dataDxfId="153"/>
-    <tableColumn id="7" xr3:uid="{49A6667C-83D4-4F03-9106-AB0608531672}" name="PrivateNetwork" dataDxfId="152"/>
-    <tableColumn id="8" xr3:uid="{EAFB87E3-07E7-4775-B47E-180417067E4A}" name="PreferredBandwidth" dataDxfId="151"/>
-    <tableColumn id="9" xr3:uid="{754AAC91-91D1-4378-9CB5-6E6BCC850CC0}" name="MaxBandwidth" dataDxfId="150"/>
-    <tableColumn id="10" xr3:uid="{3AD5FFD1-969B-4E24-88F2-117DE0453AF1}" name="UplinkSet" dataDxfId="149"/>
-    <tableColumn id="11" xr3:uid="{BE8875EA-34F5-40B2-8014-2AB67DD3D586}" name="NetworkSet" dataDxfId="148"/>
+    <tableColumn id="1" xr3:uid="{C9F95E78-00F2-4748-9AB8-00A9D57E226E}" name="Name" dataDxfId="172"/>
+    <tableColumn id="2" xr3:uid="{851B9CAB-3BBD-4E47-A479-93E1A6BB9555}" name="Purpose" dataDxfId="171"/>
+    <tableColumn id="3" xr3:uid="{A094AA9D-9339-475A-8F8A-F754CEB9212E}" name="Type" dataDxfId="170"/>
+    <tableColumn id="4" xr3:uid="{EA1F4E56-4974-4FF2-85B3-5E643B75708A}" name="VlanID" dataDxfId="169"/>
+    <tableColumn id="5" xr3:uid="{78D39E12-D3F8-4781-8503-8CC2A850C2F1}" name="IPv4Subnet" dataDxfId="168"/>
+    <tableColumn id="6" xr3:uid="{9DF7F43F-8572-4BCB-93D1-4C30EA4AD9B8}" name="Smartlink" dataDxfId="167"/>
+    <tableColumn id="7" xr3:uid="{49A6667C-83D4-4F03-9106-AB0608531672}" name="PrivateNetwork" dataDxfId="166"/>
+    <tableColumn id="8" xr3:uid="{EAFB87E3-07E7-4775-B47E-180417067E4A}" name="PreferredBandwidth" dataDxfId="165"/>
+    <tableColumn id="9" xr3:uid="{754AAC91-91D1-4378-9CB5-6E6BCC850CC0}" name="MaxBandwidth" dataDxfId="164"/>
+    <tableColumn id="10" xr3:uid="{3AD5FFD1-969B-4E24-88F2-117DE0453AF1}" name="UplinkSet" dataDxfId="163"/>
+    <tableColumn id="11" xr3:uid="{BE8875EA-34F5-40B2-8014-2AB67DD3D586}" name="NetworkSet" dataDxfId="162"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11927,13 +11927,13 @@
       <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="84.28515625" customWidth="1"/>
+    <col min="5" max="5" width="84.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12129,7 +12129,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="75">
+    <row r="15" spans="1:5" ht="72">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -13933,17 +13933,17 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="89" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" style="89" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="89" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" style="89" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="7" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+    <col min="7" max="7" width="43.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -15554,16 +15554,16 @@
       <selection pane="bottomRight" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" customWidth="1"/>
-    <col min="4" max="6" width="31.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="9" width="32.85546875" customWidth="1"/>
-    <col min="10" max="10" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.88671875" customWidth="1"/>
+    <col min="4" max="6" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.5546875" customWidth="1"/>
+    <col min="8" max="9" width="32.88671875" customWidth="1"/>
+    <col min="10" max="10" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -20148,16 +20148,16 @@
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="26.5703125" style="89" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="89" customWidth="1"/>
+    <col min="1" max="2" width="26.5546875" style="89" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="89" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
     <col min="5" max="6" width="25" style="89" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" style="89" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="89" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="89" customWidth="1"/>
+    <col min="7" max="7" width="26.44140625" style="89" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.44140625" style="89" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" style="89" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" style="89" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -20192,7 +20192,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45">
+    <row r="2" spans="1:10" ht="43.2">
       <c r="A2" s="167" t="s">
         <v>789</v>
       </c>
@@ -20230,7 +20230,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45">
+    <row r="3" spans="1:10" ht="43.2">
       <c r="A3" s="167" t="s">
         <v>789</v>
       </c>
@@ -20344,7 +20344,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="30">
+    <row r="6" spans="1:10" ht="28.8">
       <c r="A6" s="175" t="s">
         <v>789</v>
       </c>
@@ -20382,7 +20382,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30">
+    <row r="7" spans="1:10" ht="28.8">
       <c r="A7" s="167" t="s">
         <v>789</v>
       </c>
@@ -20557,7 +20557,7 @@
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
     </row>
-    <row r="13" spans="1:10" ht="45">
+    <row r="13" spans="1:10" ht="43.2">
       <c r="A13" s="58" t="s">
         <v>1061</v>
       </c>
@@ -20592,7 +20592,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30">
+    <row r="14" spans="1:10" ht="28.8">
       <c r="A14" s="58" t="s">
         <v>1061</v>
       </c>
@@ -20627,7 +20627,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="60">
+    <row r="15" spans="1:10" ht="57.6">
       <c r="A15" s="58" t="s">
         <v>1061</v>
       </c>
@@ -20662,7 +20662,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="60">
+    <row r="16" spans="1:10" ht="57.6">
       <c r="A16" s="58" t="s">
         <v>1061</v>
       </c>
@@ -20697,7 +20697,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30">
+    <row r="17" spans="1:10" ht="28.8">
       <c r="A17" s="58" t="s">
         <v>904</v>
       </c>
@@ -20732,7 +20732,7 @@
         <v>1055</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="30">
+    <row r="18" spans="1:10" ht="28.8">
       <c r="A18" s="58" t="s">
         <v>904</v>
       </c>
@@ -20802,10 +20802,10 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -20982,12 +20982,12 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="47.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="21.85546875" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -21808,11 +21808,11 @@
       <selection pane="topRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="91.5703125" customWidth="1"/>
+    <col min="1" max="1" width="91.5546875" customWidth="1"/>
     <col min="2" max="2" width="72" customWidth="1"/>
-    <col min="3" max="4" width="35.28515625" customWidth="1"/>
+    <col min="3" max="4" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -22131,11 +22131,11 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" customWidth="1"/>
-    <col min="2" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" customWidth="1"/>
+    <col min="2" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
     <col min="6" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -22634,24 +22634,24 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C123FC9F-23EA-4F5F-A4E7-231974F9FE8E}">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -23163,6 +23163,19 @@
       </c>
       <c r="K14" s="183"/>
       <c r="L14" s="183"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" s="183"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="183"/>
+      <c r="E15" s="183"/>
+      <c r="F15" s="183"/>
+      <c r="G15" s="183"/>
+      <c r="H15" s="183"/>
+      <c r="I15" s="183"/>
+      <c r="J15" s="183"/>
+      <c r="K15" s="183"/>
+      <c r="L15" s="183"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -23181,17 +23194,17 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="183" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="183" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="183"/>
-    <col min="4" max="4" width="12.42578125" style="183" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.42578125" style="183" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="183" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" style="183" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.42578125" style="183" customWidth="1"/>
-    <col min="11" max="12" width="14.42578125" style="183" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" style="183" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="183" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" style="183"/>
+    <col min="4" max="4" width="12.44140625" style="183" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.44140625" style="183" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="183" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.44140625" style="183" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.44140625" style="183" customWidth="1"/>
+    <col min="11" max="12" width="14.44140625" style="183" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -23641,24 +23654,24 @@
   </sheetPr>
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
+    <row r="1" spans="1:3" ht="18">
       <c r="A1" s="207" t="s">
         <v>1280</v>
       </c>
@@ -23765,7 +23778,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1">
+    <row r="15" spans="1:3" ht="15" thickBot="1">
       <c r="A15" s="165" t="s">
         <v>1298</v>
       </c>
@@ -23773,7 +23786,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15.75">
+    <row r="18" spans="1:7" ht="15.6">
       <c r="A18" s="189" t="s">
         <v>1723</v>
       </c>
@@ -23824,7 +23837,7 @@
         <v>1762</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15.75">
+    <row r="22" spans="1:7" ht="15.6">
       <c r="A22" s="189" t="s">
         <v>1730</v>
       </c>
@@ -23853,7 +23866,7 @@
         <v>1739</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75">
+    <row r="26" spans="1:7" ht="15.6">
       <c r="A26" s="189" t="s">
         <v>1732</v>
       </c>
@@ -23879,7 +23892,7 @@
         <v>1306</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15.75">
+    <row r="31" spans="1:7" ht="15.6">
       <c r="A31" s="189" t="s">
         <v>1308</v>
       </c>
@@ -24200,10 +24213,10 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="1" max="2" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -24379,15 +24392,15 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75">
+    <row r="1" spans="1:10" ht="18">
       <c r="A1" s="193" t="s">
         <v>1377</v>
       </c>
@@ -24559,7 +24572,7 @@
       <c r="I10" s="75"/>
       <c r="J10" s="75"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1">
+    <row r="11" spans="1:10" ht="15" thickBot="1">
       <c r="A11" s="196" t="s">
         <v>1752</v>
       </c>
@@ -24577,7 +24590,7 @@
       <c r="I11" s="75"/>
       <c r="J11" s="75"/>
     </row>
-    <row r="12" spans="1:10" ht="18.75">
+    <row r="12" spans="1:10" ht="18">
       <c r="A12" s="190" t="s">
         <v>1386</v>
       </c>
@@ -24760,7 +24773,7 @@
       <c r="F25" s="75"/>
       <c r="G25" s="75"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+    <row r="26" spans="1:10" ht="15" thickBot="1">
       <c r="A26" s="165" t="s">
         <v>1749</v>
       </c>
@@ -24775,7 +24788,7 @@
       <c r="F26" s="196"/>
       <c r="G26" s="75"/>
     </row>
-    <row r="27" spans="1:10" ht="18.75">
+    <row r="27" spans="1:10" ht="18">
       <c r="A27" s="190" t="s">
         <v>1399</v>
       </c>
@@ -24810,7 +24823,7 @@
       <c r="F29" s="75"/>
       <c r="G29" s="75"/>
     </row>
-    <row r="30" spans="1:10" ht="18.75">
+    <row r="30" spans="1:10" ht="18">
       <c r="A30" s="197" t="s">
         <v>1400</v>
       </c>
@@ -24921,12 +24934,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="1" max="4" width="30.6640625" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -25960,12 +25973,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.140625" style="75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" style="75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="103" style="75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" style="75" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="75"/>
+    <col min="4" max="16384" width="11.44140625" style="75"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -25978,7 +25991,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="408.95" customHeight="1">
+    <row r="4" spans="1:3" ht="408.9" customHeight="1">
       <c r="A4" s="214" t="s">
         <v>1406</v>
       </c>
@@ -26142,21 +26155,21 @@
       <selection pane="topRight" activeCell="A14" sqref="A14:B86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="2" max="4" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="16" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="39.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="2" max="4" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="41.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27">
@@ -28905,13 +28918,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="66.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="66.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -29167,7 +29180,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="60">
+    <row r="26" spans="1:5" ht="57.6">
       <c r="A26" s="22" t="s">
         <v>1582</v>
       </c>
@@ -29184,7 +29197,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="60">
+    <row r="27" spans="1:5" ht="57.6">
       <c r="A27" s="22" t="s">
         <v>1584</v>
       </c>
@@ -29210,7 +29223,7 @@
       <c r="D28" s="24"/>
       <c r="E28" s="24"/>
     </row>
-    <row r="29" spans="1:5" ht="60">
+    <row r="29" spans="1:5" ht="57.6">
       <c r="A29" s="22" t="s">
         <v>1587</v>
       </c>
@@ -29227,7 +29240,7 @@
         <v>1588</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="60">
+    <row r="30" spans="1:5" ht="57.6">
       <c r="A30" s="22" t="s">
         <v>1589</v>
       </c>
@@ -29253,7 +29266,7 @@
       <c r="D31" s="24"/>
       <c r="E31" s="24"/>
     </row>
-    <row r="32" spans="1:5" ht="120">
+    <row r="32" spans="1:5" ht="115.2">
       <c r="A32" s="22" t="s">
         <v>1592</v>
       </c>
@@ -29270,7 +29283,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="60">
+    <row r="33" spans="1:5" ht="57.6">
       <c r="A33" s="22" t="s">
         <v>1595</v>
       </c>
@@ -29287,7 +29300,7 @@
         <v>1583</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="30">
+    <row r="34" spans="1:5" ht="28.8">
       <c r="A34" s="23" t="s">
         <v>1596</v>
       </c>
@@ -29304,7 +29317,7 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="30">
+    <row r="35" spans="1:5" ht="28.8">
       <c r="A35" s="22" t="s">
         <v>1601</v>
       </c>
@@ -29436,13 +29449,13 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="104.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="104.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1">
@@ -29456,7 +29469,7 @@
         <v>1615</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+    <row r="2" spans="1:5" ht="15" thickTop="1">
       <c r="A2" t="s">
         <v>1616</v>
       </c>
@@ -29593,14 +29606,14 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" style="89" customWidth="1"/>
-    <col min="5" max="5" width="106.140625" customWidth="1"/>
-    <col min="6" max="6" width="75.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="52.109375" customWidth="1"/>
+    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" style="89" customWidth="1"/>
+    <col min="5" max="5" width="106.109375" customWidth="1"/>
+    <col min="6" max="6" width="75.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" thickBot="1">
@@ -29620,7 +29633,7 @@
       <c r="F1" s="100"/>
       <c r="G1" s="100"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1">
+    <row r="2" spans="1:7" ht="15" thickTop="1">
       <c r="A2" t="s">
         <v>1621</v>
       </c>
@@ -30064,13 +30077,13 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" thickBot="1">
@@ -30091,7 +30104,7 @@
       </c>
       <c r="F1" s="100"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickTop="1">
+    <row r="2" spans="1:6" ht="15" thickTop="1">
       <c r="A2" t="s">
         <v>1628</v>
       </c>
@@ -30607,12 +30620,12 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="5" width="100.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="5" width="100.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1">
@@ -30628,7 +30641,7 @@
         <v>1656</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickTop="1">
+    <row r="2" spans="1:5" ht="15" thickTop="1">
       <c r="A2" t="s">
         <v>1657</v>
       </c>
@@ -30824,20 +30837,20 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="2.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.5546875" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="4" width="2.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
     <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
     <col min="8" max="8" width="3" style="89" customWidth="1"/>
     <col min="9" max="9" width="3" customWidth="1"/>
     <col min="10" max="10" width="79" customWidth="1"/>
     <col min="11" max="11" width="50" customWidth="1"/>
-    <col min="12" max="12" width="48.28515625" customWidth="1"/>
+    <col min="12" max="12" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="100" customFormat="1" ht="18" thickBot="1">
@@ -30864,7 +30877,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" thickTop="1">
+    <row r="2" spans="1:13" ht="15" thickTop="1">
       <c r="A2" t="s">
         <v>1664</v>
       </c>
@@ -32096,10 +32109,10 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="7" width="30.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="1" max="7" width="30.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -32158,7 +32171,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="60">
+    <row r="7" spans="1:12" ht="57.6">
       <c r="A7" s="91" t="s">
         <v>61</v>
       </c>
@@ -32198,7 +32211,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="30">
+    <row r="9" spans="1:12" ht="28.8">
       <c r="A9" s="91" t="s">
         <v>73</v>
       </c>
@@ -32218,7 +32231,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30">
+    <row r="10" spans="1:12" ht="28.8">
       <c r="A10" s="91" t="s">
         <v>78</v>
       </c>
@@ -33037,14 +33050,14 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" customWidth="1"/>
+    <col min="2" max="2" width="44.5546875" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1">
+    <row r="1" spans="1:3" ht="20.399999999999999" thickBot="1">
       <c r="A1" s="181" t="s">
         <v>183</v>
       </c>
@@ -33055,7 +33068,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1">
+    <row r="2" spans="1:3" ht="15" thickTop="1">
       <c r="A2" t="s">
         <v>186</v>
       </c>
@@ -33312,23 +33325,23 @@
       <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="58" customWidth="1"/>
-    <col min="3" max="3" width="16.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" style="58" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="58" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" style="58" customWidth="1"/>
-    <col min="7" max="7" width="29.85546875" style="58" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="16.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="16.140625" style="58" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5703125" style="58" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="58"/>
+    <col min="1" max="1" width="33.88671875" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" style="58" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" style="58" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="58" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" style="58" customWidth="1"/>
+    <col min="7" max="7" width="29.88671875" style="58" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="16.33203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" style="58" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="16.109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5546875" style="58" customWidth="1"/>
+    <col min="15" max="16384" width="11.44140625" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="45">
+    <row r="1" spans="1:14" ht="43.2">
       <c r="A1" s="57" t="s">
         <v>215</v>
       </c>
@@ -33563,7 +33576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="30">
+    <row r="8" spans="1:14" ht="28.8">
       <c r="A8" s="65" t="s">
         <v>252</v>
       </c>
@@ -33876,7 +33889,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="47.25">
+    <row r="19" spans="1:14" ht="46.8">
       <c r="A19" s="66" t="s">
         <v>290</v>
       </c>
@@ -33920,7 +33933,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15.75">
+    <row r="20" spans="1:14" ht="15.6">
       <c r="A20" s="68" t="s">
         <v>227</v>
       </c>
@@ -33962,7 +33975,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="31.5">
+    <row r="21" spans="1:14" ht="31.2">
       <c r="A21" s="72" t="s">
         <v>305</v>
       </c>
@@ -34004,7 +34017,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="31.5">
+    <row r="22" spans="1:14" ht="31.2">
       <c r="A22" s="72" t="s">
         <v>235</v>
       </c>
@@ -34046,7 +34059,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15.75">
+    <row r="23" spans="1:14" ht="15.6">
       <c r="A23" s="68" t="s">
         <v>239</v>
       </c>
@@ -34088,7 +34101,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15.75">
+    <row r="24" spans="1:14" ht="15.6">
       <c r="A24" s="68" t="s">
         <v>244</v>
       </c>
@@ -34130,7 +34143,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15.75">
+    <row r="25" spans="1:14" ht="15.6">
       <c r="A25" s="68" t="s">
         <v>248</v>
       </c>
@@ -34172,7 +34185,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="31.5">
+    <row r="26" spans="1:14" ht="31.2">
       <c r="A26" s="73" t="s">
         <v>252</v>
       </c>
@@ -34214,7 +34227,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15.75">
+    <row r="27" spans="1:14" ht="15.6">
       <c r="A27" s="68" t="s">
         <v>264</v>
       </c>
@@ -34256,7 +34269,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15.75">
+    <row r="28" spans="1:14" ht="15.6">
       <c r="A28" s="68" t="s">
         <v>256</v>
       </c>
@@ -34298,7 +34311,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15.75">
+    <row r="29" spans="1:14" ht="15.6">
       <c r="A29" s="68" t="s">
         <v>268</v>
       </c>
@@ -34340,7 +34353,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15.75">
+    <row r="30" spans="1:14" ht="15.6">
       <c r="A30" s="68" t="s">
         <v>260</v>
       </c>
@@ -34382,7 +34395,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15.75">
+    <row r="31" spans="1:14" ht="15.6">
       <c r="A31" s="68" t="s">
         <v>308</v>
       </c>
@@ -34424,7 +34437,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15.75">
+    <row r="32" spans="1:14" ht="15.6">
       <c r="A32" s="68" t="s">
         <v>281</v>
       </c>
@@ -34514,7 +34527,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="30">
+    <row r="37" spans="1:14" ht="28.8">
       <c r="A37" s="74" t="s">
         <v>321</v>
       </c>
@@ -34552,7 +34565,7 @@
         <v>2550</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="30">
+    <row r="38" spans="1:14" ht="28.8">
       <c r="A38" s="74" t="s">
         <v>328</v>
       </c>
@@ -34590,7 +34603,7 @@
         <v>2551</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="30">
+    <row r="39" spans="1:14" ht="28.8">
       <c r="A39" s="74" t="s">
         <v>333</v>
       </c>
@@ -34628,7 +34641,7 @@
         <v>2552</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="30">
+    <row r="40" spans="1:14" ht="28.8">
       <c r="A40" s="74" t="s">
         <v>338</v>
       </c>
@@ -34666,7 +34679,7 @@
         <v>2553</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="30">
+    <row r="41" spans="1:14" ht="28.8">
       <c r="A41" s="74" t="s">
         <v>343</v>
       </c>
@@ -34704,7 +34717,7 @@
         <v>2554</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="30">
+    <row r="42" spans="1:14" ht="28.8">
       <c r="A42" s="74" t="s">
         <v>349</v>
       </c>
@@ -34742,7 +34755,7 @@
         <v>2555</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="30">
+    <row r="43" spans="1:14" ht="28.8">
       <c r="A43" s="74" t="s">
         <v>354</v>
       </c>
@@ -34780,7 +34793,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="30">
+    <row r="44" spans="1:14" ht="28.8">
       <c r="A44" s="74" t="s">
         <v>359</v>
       </c>
@@ -34818,7 +34831,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="30">
+    <row r="45" spans="1:14" ht="28.8">
       <c r="A45" s="74" t="s">
         <v>115</v>
       </c>
@@ -34856,7 +34869,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="30">
+    <row r="46" spans="1:14" ht="28.8">
       <c r="A46" s="74" t="s">
         <v>123</v>
       </c>
@@ -34894,7 +34907,7 @@
         <v>2101</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="30">
+    <row r="47" spans="1:14" ht="28.8">
       <c r="A47" s="74" t="s">
         <v>128</v>
       </c>
@@ -34932,7 +34945,7 @@
         <v>2102</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="30">
+    <row r="48" spans="1:14" ht="28.8">
       <c r="A48" s="74" t="s">
         <v>133</v>
       </c>
@@ -34970,7 +34983,7 @@
         <v>2103</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="30">
+    <row r="49" spans="1:14" ht="28.8">
       <c r="A49" s="74" t="s">
         <v>137</v>
       </c>
@@ -35008,7 +35021,7 @@
         <v>2104</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="30">
+    <row r="50" spans="1:14" ht="28.8">
       <c r="A50" s="74" t="s">
         <v>141</v>
       </c>
@@ -35046,7 +35059,7 @@
         <v>2105</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="30">
+    <row r="51" spans="1:14" ht="28.8">
       <c r="A51" s="74" t="s">
         <v>145</v>
       </c>
@@ -35084,7 +35097,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="30">
+    <row r="52" spans="1:14" ht="28.8">
       <c r="A52" s="81" t="s">
         <v>149</v>
       </c>
@@ -35125,7 +35138,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="30">
+    <row r="53" spans="1:14" ht="28.8">
       <c r="A53" s="81" t="s">
         <v>154</v>
       </c>
@@ -35166,7 +35179,7 @@
         <v>12.14</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="30">
+    <row r="54" spans="1:14" ht="28.8">
       <c r="A54" s="81" t="s">
         <v>159</v>
       </c>
@@ -35207,7 +35220,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="30">
+    <row r="55" spans="1:14" ht="28.8">
       <c r="A55" s="74" t="s">
         <v>163</v>
       </c>
@@ -35245,7 +35258,7 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="30">
+    <row r="56" spans="1:14" ht="28.8">
       <c r="A56" s="74" t="s">
         <v>167</v>
       </c>
@@ -35283,7 +35296,7 @@
         <v>2111</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="30">
+    <row r="57" spans="1:14" ht="28.8">
       <c r="A57" s="74" t="s">
         <v>171</v>
       </c>
@@ -35321,7 +35334,7 @@
         <v>2112</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="30">
+    <row r="58" spans="1:14" ht="28.8">
       <c r="A58" s="74" t="s">
         <v>175</v>
       </c>
@@ -35359,7 +35372,7 @@
         <v>2113</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="30">
+    <row r="59" spans="1:14" ht="28.8">
       <c r="A59" s="74" t="s">
         <v>416</v>
       </c>
@@ -35400,7 +35413,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="30">
+    <row r="60" spans="1:14" ht="28.8">
       <c r="A60" s="74" t="s">
         <v>421</v>
       </c>
@@ -35429,7 +35442,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="30">
+    <row r="61" spans="1:14" ht="28.8">
       <c r="A61" s="74" t="s">
         <v>426</v>
       </c>
@@ -35467,7 +35480,7 @@
         <v>2116</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="30">
+    <row r="62" spans="1:14" ht="28.8">
       <c r="A62" s="74" t="s">
         <v>432</v>
       </c>
@@ -35496,7 +35509,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="30">
+    <row r="63" spans="1:14" ht="28.8">
       <c r="A63" s="74" t="s">
         <v>437</v>
       </c>
@@ -35525,7 +35538,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="30">
+    <row r="64" spans="1:14" ht="28.8">
       <c r="A64" s="74" t="s">
         <v>442</v>
       </c>
@@ -35554,7 +35567,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="30">
+    <row r="65" spans="1:14" ht="28.8">
       <c r="A65" s="74" t="s">
         <v>447</v>
       </c>
@@ -35583,7 +35596,7 @@
         <v>2121</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="30">
+    <row r="66" spans="1:14" ht="28.8">
       <c r="A66" s="74" t="s">
         <v>452</v>
       </c>
@@ -35612,7 +35625,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="30">
+    <row r="67" spans="1:14" ht="28.8">
       <c r="A67" s="74" t="s">
         <v>457</v>
       </c>
@@ -35641,7 +35654,7 @@
         <v>2123</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="30">
+    <row r="68" spans="1:14" ht="28.8">
       <c r="A68" s="74" t="s">
         <v>462</v>
       </c>
@@ -35670,7 +35683,7 @@
         <v>2124</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="30">
+    <row r="69" spans="1:14" ht="28.8">
       <c r="A69" s="74" t="s">
         <v>467</v>
       </c>
@@ -35699,7 +35712,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="30">
+    <row r="70" spans="1:14" ht="28.8">
       <c r="A70" s="74" t="s">
         <v>472</v>
       </c>
@@ -35728,7 +35741,7 @@
         <v>2126</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="30">
+    <row r="71" spans="1:14" ht="28.8">
       <c r="A71" s="74" t="s">
         <v>477</v>
       </c>
@@ -35757,7 +35770,7 @@
         <v>2127</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="30">
+    <row r="72" spans="1:14" ht="28.8">
       <c r="A72" s="74" t="s">
         <v>482</v>
       </c>
@@ -35786,7 +35799,7 @@
         <v>2128</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="30">
+    <row r="73" spans="1:14" ht="28.8">
       <c r="A73" s="74" t="s">
         <v>487</v>
       </c>
@@ -35863,7 +35876,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="30">
+    <row r="76" spans="1:14" ht="28.8">
       <c r="A76" s="74" t="s">
         <v>492</v>
       </c>
@@ -35904,7 +35917,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="30">
+    <row r="77" spans="1:14" ht="28.8">
       <c r="A77" s="74" t="s">
         <v>498</v>
       </c>
@@ -35945,7 +35958,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="30">
+    <row r="78" spans="1:14" ht="28.8">
       <c r="A78" s="74" t="s">
         <v>505</v>
       </c>
@@ -35971,7 +35984,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="30">
+    <row r="79" spans="1:14" ht="28.8">
       <c r="A79" s="74" t="s">
         <v>510</v>
       </c>
@@ -35997,7 +36010,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="30">
+    <row r="80" spans="1:14" ht="28.8">
       <c r="A80" s="74" t="s">
         <v>515</v>
       </c>
@@ -36023,7 +36036,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="30">
+    <row r="81" spans="1:14" ht="28.8">
       <c r="A81" s="74" t="s">
         <v>520</v>
       </c>
@@ -36049,7 +36062,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="30">
+    <row r="82" spans="1:14" ht="28.8">
       <c r="A82" s="74" t="s">
         <v>525</v>
       </c>
@@ -36075,7 +36088,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="30">
+    <row r="83" spans="1:14" ht="28.8">
       <c r="A83" s="74" t="s">
         <v>530</v>
       </c>
@@ -36142,7 +36155,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="30">
+    <row r="86" spans="1:14" ht="28.8">
       <c r="A86" s="62" t="s">
         <v>535</v>
       </c>
@@ -36183,7 +36196,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="30">
+    <row r="87" spans="1:14" ht="28.8">
       <c r="A87" s="62" t="s">
         <v>541</v>
       </c>
@@ -36265,7 +36278,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="30">
+    <row r="90" spans="1:14" ht="28.8">
       <c r="A90" s="62" t="s">
         <v>548</v>
       </c>
@@ -36306,7 +36319,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="30">
+    <row r="91" spans="1:14" ht="28.8">
       <c r="A91" s="62" t="s">
         <v>554</v>
       </c>
@@ -36492,7 +36505,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="30">
+    <row r="104" spans="1:14" ht="28.8">
       <c r="A104" s="58" t="s">
         <v>566</v>
       </c>
@@ -36571,7 +36584,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="30">
+    <row r="107" spans="1:14" ht="28.8">
       <c r="A107" s="58" t="s">
         <v>574</v>
       </c>
@@ -36650,7 +36663,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="30">
+    <row r="110" spans="1:14" ht="28.8">
       <c r="A110" s="58" t="s">
         <v>579</v>
       </c>
@@ -36729,7 +36742,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="30">
+    <row r="113" spans="1:14" ht="28.8">
       <c r="A113" s="58" t="s">
         <v>584</v>
       </c>
@@ -36808,7 +36821,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="30">
+    <row r="116" spans="1:14" ht="28.8">
       <c r="A116" s="58" t="s">
         <v>590</v>
       </c>
@@ -36887,7 +36900,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="30">
+    <row r="119" spans="1:14" ht="28.8">
       <c r="A119" s="58" t="s">
         <v>596</v>
       </c>
@@ -36966,7 +36979,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="30">
+    <row r="122" spans="1:14" ht="28.8">
       <c r="A122" s="58" t="s">
         <v>601</v>
       </c>
@@ -37018,16 +37031,16 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="24.75" customHeight="1">
@@ -37056,7 +37069,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30">
+    <row r="2" spans="1:8" ht="28.8">
       <c r="A2" s="203" t="s">
         <v>615</v>
       </c>
@@ -37082,7 +37095,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8" ht="28.8">
       <c r="A3" s="203"/>
       <c r="B3" s="152">
         <v>2501</v>
@@ -37106,7 +37119,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30">
+    <row r="4" spans="1:8" ht="28.8">
       <c r="A4" s="203"/>
       <c r="B4" s="152">
         <v>2502</v>
@@ -37130,7 +37143,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30">
+    <row r="5" spans="1:8" ht="28.8">
       <c r="A5" s="203"/>
       <c r="B5" s="152">
         <v>2503</v>
@@ -37154,7 +37167,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30">
+    <row r="6" spans="1:8" ht="28.8">
       <c r="A6" s="203"/>
       <c r="B6" s="152">
         <v>2504</v>
@@ -37178,7 +37191,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30">
+    <row r="7" spans="1:8" ht="28.8">
       <c r="A7" s="203"/>
       <c r="B7" s="152">
         <v>2505</v>
@@ -37202,7 +37215,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30">
+    <row r="8" spans="1:8" ht="28.8">
       <c r="A8" s="203"/>
       <c r="B8" s="152">
         <v>2506</v>
@@ -37226,7 +37239,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30">
+    <row r="9" spans="1:8" ht="28.8">
       <c r="A9" s="203"/>
       <c r="B9" s="152">
         <v>2507</v>
@@ -37250,7 +37263,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="30">
+    <row r="10" spans="1:8">
       <c r="A10" s="204"/>
       <c r="B10" s="152">
         <v>2549</v>
@@ -37274,7 +37287,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="30">
+    <row r="11" spans="1:8" ht="28.8">
       <c r="A11" s="203" t="s">
         <v>663</v>
       </c>
@@ -37300,7 +37313,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:8" ht="28.8">
       <c r="A12" s="203"/>
       <c r="B12" s="152">
         <v>2551</v>
@@ -37324,7 +37337,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="30">
+    <row r="13" spans="1:8" ht="28.8">
       <c r="A13" s="203"/>
       <c r="B13" s="152">
         <v>2552</v>
@@ -37348,7 +37361,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30">
+    <row r="14" spans="1:8" ht="28.8">
       <c r="A14" s="203"/>
       <c r="B14" s="152">
         <v>2553</v>
@@ -37372,7 +37385,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="30">
+    <row r="15" spans="1:8" ht="28.8">
       <c r="A15" s="203"/>
       <c r="B15" s="152">
         <v>2554</v>
@@ -37396,7 +37409,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30">
+    <row r="16" spans="1:8" ht="28.8">
       <c r="A16" s="203"/>
       <c r="B16" s="152">
         <v>2555</v>
@@ -37420,7 +37433,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="30">
+    <row r="17" spans="1:8" ht="28.8">
       <c r="A17" s="203"/>
       <c r="B17" s="152">
         <v>2556</v>
@@ -37444,7 +37457,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30">
+    <row r="18" spans="1:8" ht="28.8">
       <c r="A18" s="205"/>
       <c r="B18" s="152">
         <v>2557</v>
@@ -37782,13 +37795,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -38063,10 +38076,10 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -38194,11 +38207,11 @@
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
   </cols>
@@ -38340,11 +38353,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_Flow_SignoffStatus xmlns="eaf262ef-7826-430c-9070-0dd2e6d0c7a3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -38524,26 +38538,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_Flow_SignoffStatus xmlns="eaf262ef-7826-430c-9070-0dd2e6d0c7a3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C87939E5-2E1D-451A-AA58-3A58F63DCD26}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6A03F3-6EBC-493D-9331-FC3669ADBF91}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="eaf262ef-7826-430c-9070-0dd2e6d0c7a3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -38567,9 +38572,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF6A03F3-6EBC-493D-9331-FC3669ADBF91}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C87939E5-2E1D-451A-AA58-3A58F63DCD26}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="eaf262ef-7826-430c-9070-0dd2e6d0c7a3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>